<commit_message>
Test + Yorum Satırlarının Eklenmesi
Co-Authored-By: Selencalk <149872006+Selencalk@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Tablolar/Tablo 1.xlsx
+++ b/Tablolar/Tablo 1.xlsx
@@ -1,29 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45CE053-196C-484C-96F2-78D690340940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Tablo 1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Tablo 1" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -72,14 +55,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -445,19 +428,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="7" width="35" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,152 +458,86 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1">
-        <f t="shared" ref="G2:G7" si="0">SUM(B2:F2) / COUNTA(B2:F2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+        <f>SUM(B2:F2) / COUNTA(B2:F2)</f>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+        <f>SUM(B3:F3) / COUNTA(B3:F3)</f>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+        <f>SUM(B4:F4) / COUNTA(B4:F4)</f>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+        <f>SUM(B5:F5) / COUNTA(B5:F5)</f>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <f>SUM(B6:F6) / COUNTA(B6:F6)</f>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
+        <f>SUM(B7:F7) / COUNTA(B7:F7)</f>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>